<commit_message>
sakshisarve: Hlookup and document added for Hlookup and Vlookup
</commit_message>
<xml_diff>
--- a/day-12.xlsx
+++ b/day-12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5743ee7966fd660a/Documents/Data Analytics/Day 12/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="411" documentId="13_ncr:1_{9DAE0993-5FAA-45CF-9CE9-5F4E53E2D00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACA1B69C-E4ED-4258-8A59-B195F5C23317}"/>
+  <xr:revisionPtr revIDLastSave="471" documentId="13_ncr:1_{9DAE0993-5FAA-45CF-9CE9-5F4E53E2D00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75D91454-B9BA-4FFB-BB84-DFF1B94F1515}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example 1" sheetId="14" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="98">
   <si>
     <t>dmart</t>
   </si>
@@ -453,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -462,6 +462,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -476,7 +479,12 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,14 +765,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A40DD5A-2EA0-453B-B205-8D25B7B6EF10}">
-  <dimension ref="D3:J22"/>
+  <dimension ref="D3:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="170" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="5.21875" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
@@ -772,18 +783,19 @@
     <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D3" s="6" t="s">
+    <row r="3" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="5" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
@@ -806,7 +818,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="4:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D6" s="2" t="s">
         <v>0</v>
       </c>
@@ -831,7 +843,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D7" s="2" t="s">
         <v>1</v>
       </c>
@@ -856,7 +868,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D8" s="2" t="s">
         <v>2</v>
       </c>
@@ -881,7 +893,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D9" s="2" t="s">
         <v>3</v>
       </c>
@@ -906,7 +918,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D10" s="2" t="s">
         <v>4</v>
       </c>
@@ -931,7 +943,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D11" s="2" t="s">
         <v>5</v>
       </c>
@@ -956,7 +968,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D14" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D15">
         <v>1</v>
       </c>
@@ -964,7 +984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
@@ -974,8 +994,20 @@
       <c r="F16" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="H16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D17" s="2" t="s">
         <v>3</v>
       </c>
@@ -985,8 +1017,23 @@
       <c r="F17" s="2">
         <v>200000</v>
       </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="H17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" t="str">
+        <f>HLOOKUP(I16,$D$5:$J$11,3,FALSE)</f>
+        <v>offline</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ref="J17:K17" si="0">HLOOKUP(J16,$D$5:$J$11,3,FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D18" s="2" t="s">
         <v>5</v>
       </c>
@@ -996,8 +1043,23 @@
       <c r="F18" s="2">
         <v>50000</v>
       </c>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="H18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" t="str">
+        <f>HLOOKUP(I16,$D$5:$J$11,6,FALSE)</f>
+        <v>online</v>
+      </c>
+      <c r="J18">
+        <f t="shared" ref="J18:K18" si="1">HLOOKUP(J16,$D$5:$J$11,6,FALSE)</f>
+        <v>7000</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D19" s="2" t="s">
         <v>2</v>
       </c>
@@ -1008,7 +1070,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D20" s="2" t="s">
         <v>0</v>
       </c>
@@ -1019,7 +1081,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D21" s="2" t="s">
         <v>4</v>
       </c>
@@ -1030,7 +1092,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D22" s="2" t="s">
         <v>1</v>
       </c>
@@ -1053,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F17580ED-6481-4B8A-9478-5ED876956F77}">
   <dimension ref="C4:I28"/>
   <sheetViews>
-    <sheetView zoomScale="126" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A2" zoomScale="126" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1237,10 +1299,10 @@
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="8"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C14" s="5" t="s">
@@ -1312,7 +1374,7 @@
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1415,29 +1477,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF3A4E4B-3756-4E51-A307-A259F24638A3}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView zoomScale="152" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1454,7 +1518,7 @@
       <c r="D2" s="4">
         <v>50000</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1485,16 +1549,16 @@
       <c r="D4" s="4">
         <v>60000</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="10" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1655,6 +1719,9 @@
       <c r="D11" s="4">
         <v>33000</v>
       </c>
+      <c r="F11" s="17" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -1683,6 +1750,15 @@
       <c r="D13" s="4">
         <v>50000</v>
       </c>
+      <c r="F13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -1697,6 +1773,17 @@
       <c r="D14" s="4">
         <v>50000</v>
       </c>
+      <c r="F14" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="6" t="str">
+        <f>HLOOKUP(F14,$A$1:$D$15,2,FALSE)</f>
+        <v xml:space="preserve">Rajashree vyas </v>
+      </c>
+      <c r="H14" s="6" t="str">
+        <f>HLOOKUP(F14,$A$1:$D$15,12,FALSE)</f>
+        <v xml:space="preserve">khushi shinde </v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
@@ -1710,6 +1797,30 @@
       </c>
       <c r="D15" s="4">
         <v>45000</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" ref="G15:G16" si="3">HLOOKUP(F15,$A$1:$D$15,2,FALSE)</f>
+        <v>50000</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" ref="H15:H16" si="4">HLOOKUP(F15,$A$1:$D$15,12,FALSE)</f>
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Sales</v>
+      </c>
+      <c r="H16" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">Operations </v>
       </c>
     </row>
   </sheetData>
@@ -1723,7 +1834,7 @@
   <dimension ref="A2:K13"/>
   <sheetViews>
     <sheetView zoomScale="141" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1731,75 +1842,76 @@
     <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+      <c r="A4" s="13">
         <v>101</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="13">
         <v>88</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="13">
         <v>78</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="13">
         <f>C4+D4</f>
         <v>166</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
+      <c r="A5" s="13">
         <v>102</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="13">
         <v>90</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="13">
         <v>56</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="13">
         <f t="shared" ref="E5:E13" si="0">C5+D5</f>
         <v>146</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="13">
         <v>101</v>
       </c>
       <c r="H5" t="str">
@@ -1812,23 +1924,23 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
+      <c r="A6" s="13">
         <v>103</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="13">
         <v>66</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="13">
         <v>88</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="13">
         <f t="shared" si="0"/>
         <v>154</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="13">
         <v>104</v>
       </c>
       <c r="H6" t="str">
@@ -1841,23 +1953,23 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
+      <c r="A7" s="13">
         <v>104</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="13">
         <v>78</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="13">
         <v>45</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="13">
         <f t="shared" si="0"/>
         <v>123</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="13">
         <v>110</v>
       </c>
       <c r="H7" t="str">
@@ -1870,149 +1982,165 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="12">
+      <c r="A8" s="13">
         <v>105</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="13">
         <v>55</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="13">
         <v>77</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="13">
         <f t="shared" si="0"/>
         <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="12">
+      <c r="A9" s="13">
         <v>106</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="13">
         <v>45</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="13">
         <v>65</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="13">
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="9" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="12">
+      <c r="A10" s="13">
         <v>107</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="13">
         <v>77</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="13">
         <v>48</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="13">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="12" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="12">
+      <c r="A11" s="13">
         <v>108</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="13">
         <v>86</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="13">
         <v>79</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="13">
         <f t="shared" si="0"/>
         <v>165</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="13">
         <v>101</v>
       </c>
-      <c r="H11" t="e">
-        <f>HLOOKUP(G11,$A$3:$E$13,4,FALSE)</f>
-        <v>#N/A</v>
+      <c r="H11">
+        <f>HLOOKUP(H10,$A$3:$E$13,2,FALSE)</f>
+        <v>88</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11:K11" si="3">HLOOKUP(I10,$A$3:$E$13,4,FALSE)</f>
-        <v>88</v>
+        <f t="shared" ref="I11:K11" si="3">HLOOKUP(I10,$A$3:$E$13,2,FALSE)</f>
+        <v>78</v>
       </c>
       <c r="J11">
         <f t="shared" si="3"/>
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="3"/>
-        <v>khushi</v>
+        <v xml:space="preserve">Radha </v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="12">
+      <c r="A12" s="13">
         <v>109</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="13">
         <v>65</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="13">
         <v>56</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="13">
         <f t="shared" si="0"/>
         <v>121</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="13">
         <v>105</v>
       </c>
+      <c r="H12">
+        <f>HLOOKUP(H10,$A$3:$E$13,8,FALSE)</f>
+        <v>77</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12:K12" si="4">HLOOKUP(I10,$A$3:$E$13,8,FALSE)</f>
+        <v>48</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="4"/>
+        <v>125</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="4"/>
+        <v>Raj</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="12">
+      <c r="A13" s="13">
         <v>110</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="13">
         <v>63</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="13">
         <v>74</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="13">
         <f t="shared" si="0"/>
         <v>137</v>
       </c>
@@ -2026,8 +2154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624EF9C8-5E05-49AD-81BB-02D28AB4C4C3}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:G16"/>
+    <sheetView zoomScale="129" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2054,85 +2182,85 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="15">
         <v>10</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="15">
         <v>100</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="15">
         <v>5000</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="15">
         <v>9</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="15">
         <v>120</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="15">
         <v>6000</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="15">
         <v>12</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="15">
         <v>320</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="15">
         <v>7800</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="15" t="s">
         <v>82</v>
       </c>
       <c r="H5">
@@ -2145,22 +2273,22 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="15">
         <v>15</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="15">
         <v>200</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="15">
         <v>2400</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="15" t="s">
         <v>84</v>
       </c>
       <c r="H6">
@@ -2173,22 +2301,22 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="15">
         <v>20</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="15">
         <v>4500</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="15">
         <v>9000</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="15" t="s">
         <v>88</v>
       </c>
       <c r="H7">
@@ -2201,22 +2329,22 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="15">
         <v>7</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="15">
         <v>600</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="15">
         <v>4700</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="15" t="s">
         <v>89</v>
       </c>
       <c r="H8">
@@ -2229,78 +2357,78 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="15">
         <v>6</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="15">
         <v>740</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="15">
         <v>3000</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="15">
         <v>13</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="15">
         <v>200</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="15">
         <v>800</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="15">
         <v>16</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="15">
         <v>100</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="15">
         <v>2500</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="19" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="14" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="15" t="s">
         <v>81</v>
       </c>
       <c r="G14">
@@ -2321,44 +2449,44 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="G15" t="e">
-        <f t="shared" ref="G15:G16" si="3">HLOOKUP(G14,$A$2:$E$11,2,FALSE)</f>
-        <v>#N/A</v>
+      <c r="G15">
+        <f>HLOOKUP(G13,$A$2:$E$11,3,FALSE)</f>
+        <v>9</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:I15" si="4">HLOOKUP(H13,$A$2:$E$11,3,FALSE)</f>
+        <f t="shared" ref="H15:J15" si="3">HLOOKUP(H13,$A$2:$E$11,3,FALSE)</f>
         <v>120</v>
       </c>
       <c r="I15" t="str">
+        <f t="shared" si="3"/>
+        <v>pune</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F16" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16">
+        <f>HLOOKUP(G13,$A$2:$E$11,4,FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ref="H16:J16" si="4">HLOOKUP(H13,$A$2:$E$11,4,FALSE)</f>
+        <v>320</v>
+      </c>
+      <c r="I16" t="str">
         <f t="shared" si="4"/>
-        <v>pune</v>
-      </c>
-      <c r="J15">
-        <f>HLOOKUP(J13,$A$2:$E$11,3,FALSE)</f>
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F16" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="G16" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H16">
-        <f t="shared" ref="H16:J16" si="5">HLOOKUP(H$13,$A$2:$E$11,4,FALSE)</f>
-        <v>320</v>
-      </c>
-      <c r="I16" t="str">
-        <f t="shared" si="5"/>
         <v>Delhi</v>
       </c>
       <c r="J16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>7800</v>
       </c>
     </row>

</xml_diff>